<commit_message>
doc(backend): And some dirs changed
</commit_message>
<xml_diff>
--- a/docs/SCRUM/backlog.xlsx
+++ b/docs/SCRUM/backlog.xlsx
@@ -57,7 +57,7 @@
     <t>Medium</t>
   </si>
   <si>
-    <t>In Progress</t>
+    <t>Overdue</t>
   </si>
   <si>
     <t>Not Started</t>
@@ -78,6 +78,9 @@
     <t>Complete</t>
   </si>
   <si>
+    <t>In Progress</t>
+  </si>
+  <si>
     <t>Be able to create an account</t>
   </si>
   <si>
@@ -94,9 +97,6 @@
   </si>
   <si>
     <t>Others see my chirps</t>
-  </si>
-  <si>
-    <t>Overdue</t>
   </si>
   <si>
     <t>Send chirps with @mentions</t>
@@ -935,7 +935,7 @@
       </c>
       <c r="J5" s="6"/>
       <c r="K5" s="22" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="L5" s="6"/>
       <c r="M5" s="23" t="s">
@@ -963,10 +963,10 @@
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G6" s="17" t="s">
         <v>12</v>
@@ -975,7 +975,7 @@
         <v>2.0</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="J6" s="6"/>
       <c r="K6" s="22" t="s">
@@ -983,7 +983,7 @@
       </c>
       <c r="L6" s="6"/>
       <c r="M6" s="25" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
@@ -1003,25 +1003,25 @@
       <c r="A7" s="4"/>
       <c r="B7" s="21"/>
       <c r="C7" s="15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G7" s="17" t="s">
         <v>12</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="17" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="J7" s="6"/>
       <c r="K7" s="27" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
@@ -1043,7 +1043,7 @@
       <c r="A8" s="4"/>
       <c r="B8" s="21"/>
       <c r="C8" s="15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="16" t="s">
@@ -1053,7 +1053,7 @@
         <v>28</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H8" s="24">
         <v>3.0</v>
@@ -1093,7 +1093,7 @@
       </c>
       <c r="F9" s="28"/>
       <c r="G9" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H9" s="29"/>
       <c r="I9" s="17" t="s">
@@ -1131,7 +1131,7 @@
         <v>33</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H10" s="29"/>
       <c r="I10" s="17" t="s">
@@ -1167,7 +1167,7 @@
       </c>
       <c r="F11" s="28"/>
       <c r="G11" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="17" t="s">
@@ -1203,7 +1203,7 @@
       </c>
       <c r="F12" s="28"/>
       <c r="G12" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H12" s="18">
         <v>4.0</v>
@@ -1237,7 +1237,7 @@
       <c r="E13" s="31"/>
       <c r="F13" s="28"/>
       <c r="G13" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H13" s="32">
         <v>0.0</v>
@@ -1271,7 +1271,7 @@
       <c r="E14" s="31"/>
       <c r="F14" s="28"/>
       <c r="G14" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H14" s="32">
         <v>0.0</v>
@@ -1305,7 +1305,7 @@
       <c r="E15" s="31"/>
       <c r="F15" s="28"/>
       <c r="G15" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H15" s="32">
         <v>0.0</v>
@@ -1339,7 +1339,7 @@
       <c r="E16" s="31"/>
       <c r="F16" s="28"/>
       <c r="G16" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H16" s="32">
         <v>0.0</v>
@@ -1373,7 +1373,7 @@
       <c r="E17" s="31"/>
       <c r="F17" s="28"/>
       <c r="G17" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H17" s="32">
         <v>0.0</v>

</xml_diff>